<commit_message>
new plots for the scottish fleet
</commit_message>
<xml_diff>
--- a/Fisheries/Fisheries.xlsx
+++ b/Fisheries/Fisheries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlaleone/Desktop/Exeter/Fisheries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67FD1F92-E355-EA46-9A3E-1BA8A5AD3A7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9532F61A-6EDA-B947-B743-FADD9FF7E5A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16340" firstSheet="2" activeTab="5" xr2:uid="{07497000-BD50-6443-8FB5-C721D9BC065F}"/>
   </bookViews>
@@ -17809,161 +17809,116 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C35EF5A0-2951-6D41-BFAF-7A6804BB372F}">
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+      <selection activeCell="B1" sqref="B1:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>116</v>
       </c>
       <c r="B1">
-        <v>2009</v>
+        <v>2014</v>
       </c>
       <c r="C1">
-        <v>2010</v>
+        <v>2015</v>
       </c>
       <c r="D1">
-        <v>2011</v>
+        <v>2016</v>
       </c>
       <c r="E1">
-        <v>2012</v>
+        <v>2017</v>
       </c>
       <c r="F1">
-        <v>2013</v>
+        <v>2018</v>
       </c>
       <c r="G1">
-        <v>2014</v>
+        <v>2019</v>
       </c>
       <c r="H1">
-        <v>2015</v>
+        <v>2020</v>
       </c>
       <c r="I1">
-        <v>2016</v>
+        <v>2021</v>
       </c>
       <c r="J1">
-        <v>2017</v>
+        <v>2022</v>
       </c>
       <c r="K1">
-        <v>2018</v>
-      </c>
-      <c r="L1">
-        <v>2019</v>
-      </c>
-      <c r="M1">
-        <v>2020</v>
-      </c>
-      <c r="N1">
-        <v>2021</v>
-      </c>
-      <c r="O1">
-        <v>2022</v>
-      </c>
-      <c r="P1">
         <v>2023</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>106</v>
       </c>
       <c r="B2" s="177">
-        <v>785.67857139140062</v>
+        <v>928.37688459369997</v>
       </c>
       <c r="C2" s="177">
-        <v>827.37738979537801</v>
+        <v>835.10268893869977</v>
       </c>
       <c r="D2" s="177">
-        <v>937.33264814282586</v>
+        <v>1046.9857301541363</v>
       </c>
       <c r="E2" s="177">
-        <v>858.19700842068983</v>
+        <v>1087.3267147720283</v>
       </c>
       <c r="F2" s="177">
-        <v>827.95650277720574</v>
+        <v>1098.0439383842088</v>
       </c>
       <c r="G2" s="177">
-        <v>928.37688459369997</v>
+        <v>1168.3915416829361</v>
       </c>
       <c r="H2" s="177">
-        <v>835.10268893869977</v>
+        <v>915.7448503173722</v>
       </c>
       <c r="I2" s="177">
-        <v>1046.9857301541363</v>
+        <v>1050.6481471019144</v>
       </c>
       <c r="J2" s="177">
-        <v>1087.3267147720283</v>
+        <v>1194.5237937655736</v>
       </c>
       <c r="K2" s="177">
-        <v>1098.0439383842088</v>
-      </c>
-      <c r="L2" s="177">
-        <v>1168.3915416829361</v>
-      </c>
-      <c r="M2" s="177">
-        <v>915.7448503173722</v>
-      </c>
-      <c r="N2" s="177">
-        <v>1050.6481471019144</v>
-      </c>
-      <c r="O2" s="177">
-        <v>1194.5237937655736</v>
-      </c>
-      <c r="P2" s="177">
         <v>1231.3208478849297</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>107</v>
       </c>
       <c r="B3" s="177">
-        <v>393.42486400000013</v>
+        <v>449.15647059999986</v>
       </c>
       <c r="C3" s="177">
-        <v>408.29298139999992</v>
+        <v>415.95173549999998</v>
       </c>
       <c r="D3" s="177">
-        <v>400.12264429999999</v>
+        <v>444.38999190000015</v>
       </c>
       <c r="E3" s="177">
-        <v>393.79796019999992</v>
+        <v>433.74892149999999</v>
       </c>
       <c r="F3" s="177">
-        <v>404.64696000000004</v>
+        <v>425.99776420000001</v>
       </c>
       <c r="G3" s="177">
-        <v>449.15647059999986</v>
+        <v>393.74959581082032</v>
       </c>
       <c r="H3" s="177">
-        <v>415.95173549999998</v>
+        <v>380.2616938508412</v>
       </c>
       <c r="I3" s="177">
-        <v>444.38999190000015</v>
+        <v>395.11400356937679</v>
       </c>
       <c r="J3" s="177">
-        <v>433.74892149999999</v>
+        <v>398.19193768409707</v>
       </c>
       <c r="K3" s="177">
-        <v>425.99776420000001</v>
-      </c>
-      <c r="L3" s="177">
-        <v>393.74959581082032</v>
-      </c>
-      <c r="M3" s="177">
-        <v>380.2616938508412</v>
-      </c>
-      <c r="N3" s="177">
-        <v>395.11400356937679</v>
-      </c>
-      <c r="O3" s="177">
-        <v>398.19193768409707</v>
-      </c>
-      <c r="P3" s="177">
         <v>440.53138674432535</v>
       </c>
     </row>

</xml_diff>

<commit_message>
facet plot to clarify the value and catch for each species
</commit_message>
<xml_diff>
--- a/Fisheries/Fisheries.xlsx
+++ b/Fisheries/Fisheries.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlaleone/Desktop/Exeter/Fisheries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9532F61A-6EDA-B947-B743-FADD9FF7E5A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F63B5F53-25CD-C64E-B5B8-37F8C549EC8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16340" firstSheet="2" activeTab="5" xr2:uid="{07497000-BD50-6443-8FB5-C721D9BC065F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16340" firstSheet="2" activeTab="4" xr2:uid="{07497000-BD50-6443-8FB5-C721D9BC065F}"/>
   </bookViews>
   <sheets>
     <sheet name="Total Value" sheetId="13" r:id="rId1"/>
@@ -1543,10 +1543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44AC6F4C-D30F-DF4A-84A6-D62647040C43}">
-  <dimension ref="A1:P44"/>
+  <dimension ref="A1:S44"/>
   <sheetViews>
     <sheetView zoomScale="75" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44:P44"/>
+      <selection activeCell="R34" sqref="R34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2351,7 +2351,7 @@
         <v>17.883876766557563</v>
       </c>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:19">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -2401,7 +2401,7 @@
         <v>3.9811028897999996E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:19">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -2451,7 +2451,7 @@
         <v>6.2327460475307399</v>
       </c>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:19">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -2501,7 +2501,7 @@
         <v>36.113557174869172</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:19">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -2551,7 +2551,7 @@
         <v>8.8104264016656391</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:19">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -2601,7 +2601,7 @@
         <v>18.738675662866857</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:19">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -2651,7 +2651,7 @@
         <v>1.1258287092567612</v>
       </c>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:19">
       <c r="A23" t="s">
         <v>56</v>
       </c>
@@ -2701,7 +2701,7 @@
         <v>29.308531829515168</v>
       </c>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:19">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -2751,7 +2751,7 @@
         <v>429.83553445895006</v>
       </c>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:19">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -2801,7 +2801,7 @@
         <v>10.070873287563201</v>
       </c>
     </row>
-    <row r="26" spans="1:16">
+    <row r="26" spans="1:19">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -2851,7 +2851,7 @@
         <v>43.568628115810711</v>
       </c>
     </row>
-    <row r="27" spans="1:16">
+    <row r="27" spans="1:19">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -2901,7 +2901,7 @@
         <v>0.66396589701580255</v>
       </c>
     </row>
-    <row r="28" spans="1:16">
+    <row r="28" spans="1:19">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -2950,8 +2950,16 @@
       <c r="P28" s="177">
         <v>201.68746372075208</v>
       </c>
-    </row>
-    <row r="29" spans="1:16">
+      <c r="R28">
+        <f>((P28-G28)/G28)*100</f>
+        <v>28.330983856757204</v>
+      </c>
+      <c r="S28">
+        <f>G28*1.283</f>
+        <v>201.63876889041691</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -3001,7 +3009,7 @@
         <v>4.4907042742758003</v>
       </c>
     </row>
-    <row r="30" spans="1:16">
+    <row r="30" spans="1:19">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -3051,7 +3059,7 @@
         <v>0.66686391323619998</v>
       </c>
     </row>
-    <row r="31" spans="1:16">
+    <row r="31" spans="1:19">
       <c r="A31" t="s">
         <v>32</v>
       </c>
@@ -3101,7 +3109,7 @@
         <v>261.14849920865385</v>
       </c>
     </row>
-    <row r="32" spans="1:16">
+    <row r="32" spans="1:19">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -6217,10 +6225,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C30A5893-199B-2948-9744-2984649A120F}">
-  <dimension ref="A1:P44"/>
+  <dimension ref="A1:S44"/>
   <sheetViews>
     <sheetView zoomScale="69" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44:P44"/>
+      <selection activeCell="T28" sqref="T28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -7025,7 +7033,7 @@
         <v>9.5080807800001548</v>
       </c>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:19">
       <c r="A17" s="93" t="s">
         <v>18</v>
       </c>
@@ -7075,7 +7083,7 @@
         <v>8.5479999999999996E-4</v>
       </c>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:19">
       <c r="A18" s="93" t="s">
         <v>19</v>
       </c>
@@ -7125,7 +7133,7 @@
         <v>2.7269163920080839</v>
       </c>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:19">
       <c r="A19" s="93" t="s">
         <v>20</v>
       </c>
@@ -7175,7 +7183,7 @@
         <v>1.6218717000137139</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:19">
       <c r="A20" s="93" t="s">
         <v>21</v>
       </c>
@@ -7225,7 +7233,7 @@
         <v>0.40236944200235031</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:19">
       <c r="A21" s="93" t="s">
         <v>22</v>
       </c>
@@ -7275,7 +7283,7 @@
         <v>12.280845450000919</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:19">
       <c r="A22" s="93" t="s">
         <v>23</v>
       </c>
@@ -7325,7 +7333,7 @@
         <v>0.70467764000007305</v>
       </c>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:19">
       <c r="A23" s="85" t="s">
         <v>56</v>
       </c>
@@ -7375,7 +7383,7 @@
         <v>5.9612086290031288</v>
       </c>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:19">
       <c r="A24" s="97" t="s">
         <v>25</v>
       </c>
@@ -7425,7 +7433,7 @@
         <v>128.38383882427257</v>
       </c>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:19">
       <c r="A25" s="93" t="s">
         <v>26</v>
       </c>
@@ -7475,7 +7483,7 @@
         <v>26.8770442</v>
       </c>
     </row>
-    <row r="26" spans="1:16">
+    <row r="26" spans="1:19">
       <c r="A26" s="93" t="s">
         <v>27</v>
       </c>
@@ -7525,7 +7533,7 @@
         <v>45.405696499999998</v>
       </c>
     </row>
-    <row r="27" spans="1:16">
+    <row r="27" spans="1:19">
       <c r="A27" s="93" t="s">
         <v>28</v>
       </c>
@@ -7575,7 +7583,7 @@
         <v>0.64717800000000225</v>
       </c>
     </row>
-    <row r="28" spans="1:16">
+    <row r="28" spans="1:19">
       <c r="A28" s="93" t="s">
         <v>29</v>
       </c>
@@ -7624,8 +7632,12 @@
       <c r="P28" s="7">
         <v>107.6580944</v>
       </c>
-    </row>
-    <row r="29" spans="1:16">
+      <c r="S28">
+        <f>((G28-P28)/G28)*100</f>
+        <v>14.673884602860293</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19">
       <c r="A29" s="93" t="s">
         <v>30</v>
       </c>
@@ -7675,7 +7687,7 @@
         <v>8.4491595000000004</v>
       </c>
     </row>
-    <row r="30" spans="1:16">
+    <row r="30" spans="1:19">
       <c r="A30" s="85" t="s">
         <v>31</v>
       </c>
@@ -7725,7 +7737,7 @@
         <v>0.5975916</v>
       </c>
     </row>
-    <row r="31" spans="1:16">
+    <row r="31" spans="1:19">
       <c r="A31" s="97" t="s">
         <v>32</v>
       </c>
@@ -7775,7 +7787,7 @@
         <v>189.63476420000001</v>
       </c>
     </row>
-    <row r="32" spans="1:16">
+    <row r="32" spans="1:19">
       <c r="A32" s="93" t="s">
         <v>33</v>
       </c>
@@ -15773,7 +15785,7 @@
   <dimension ref="A1:X24"/>
   <sheetViews>
     <sheetView zoomScale="87" workbookViewId="0">
-      <selection sqref="A1:N12"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -17142,8 +17154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46CBB3C8-6CD7-8142-9B6C-C07F765CBF57}">
   <dimension ref="A1:W24"/>
   <sheetViews>
-    <sheetView zoomScale="87" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" zoomScale="87" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -17645,10 +17657,19 @@
     <row r="13" spans="1:19" ht="17" thickBot="1">
       <c r="A13" s="36"/>
       <c r="B13" s="173"/>
-      <c r="C13" s="36"/>
+      <c r="C13" s="36">
+        <f>((C11-C2)/C2)*100</f>
+        <v>3.017832647462277</v>
+      </c>
       <c r="D13" s="173"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="173"/>
+      <c r="E13" s="36">
+        <f>((E11-E2)/E2)*100</f>
+        <v>12.995156871888508</v>
+      </c>
+      <c r="F13" s="36">
+        <f>((F2-F11)/F11)*100</f>
+        <v>5.834796910770959</v>
+      </c>
       <c r="G13" s="36"/>
       <c r="H13" s="36"/>
       <c r="I13" s="36"/>
@@ -17683,6 +17704,12 @@
       <c r="Q14" s="68"/>
       <c r="R14" s="172"/>
       <c r="S14" s="68"/>
+    </row>
+    <row r="15" spans="1:19">
+      <c r="F15">
+        <f>1.13*E2</f>
+        <v>122058.91620000005</v>
+      </c>
     </row>
     <row r="17" spans="1:23" ht="17" thickBot="1"/>
     <row r="18" spans="1:23" ht="17" thickBot="1">
@@ -17811,8 +17838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C35EF5A0-2951-6D41-BFAF-7A6804BB372F}">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:F3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>